<commit_message>
updates based on comments from kumar
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0FF972-DF8A-4785-A20A-B8496DE0538C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33FE740-512A-448D-ABBE-35698A71D115}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -230,6 +230,10 @@
   </si>
   <si>
     <t>price_EP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -331,7 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -351,6 +355,11 @@
     <xf numFmtId="24" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -632,89 +641,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" customWidth="1"/>
-    <col min="4" max="5" width="10.375" customWidth="1"/>
-    <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.875" customWidth="1"/>
+    <col min="5" max="6" width="10.375" customWidth="1"/>
+    <col min="7" max="7" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
         <v>24</v>
       </c>
-      <c r="C2" s="5">
+      <c r="D2" s="5">
         <v>4.5</v>
       </c>
-      <c r="D2" s="5">
+      <c r="E2" s="5">
         <v>100000</v>
       </c>
-      <c r="E2" s="9">
+      <c r="F2" s="9">
         <v>100000</v>
-      </c>
-      <c r="F2" s="9">
-        <v>0</v>
       </c>
       <c r="G2" s="9">
         <v>0</v>
@@ -725,60 +737,68 @@
       <c r="I2" s="9">
         <v>0</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="9">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="9">
+      <c r="M2" s="9">
         <v>100000</v>
       </c>
-      <c r="M2" s="10">
+      <c r="N2" s="10">
         <v>4756</v>
       </c>
-      <c r="N2" s="9">
+      <c r="O2" s="9">
         <v>104756</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="5">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>4.3</v>
+        <v>24</v>
       </c>
       <c r="D3" s="5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E3" s="5">
         <v>100000</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M3" s="9"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5">
-        <v>4.2</v>
+        <v>36</v>
       </c>
       <c r="D4" s="5">
+        <v>4.3</v>
+      </c>
+      <c r="E4" s="5">
         <v>100000</v>
       </c>
-      <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -788,21 +808,24 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5">
-        <v>4.0999999999999996</v>
+        <v>48</v>
       </c>
       <c r="D5" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="E5" s="5">
         <v>100000</v>
       </c>
-      <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -812,30 +835,67 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-    </row>
-    <row r="6" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="5">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="D6" s="5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E6" s="5">
+        <v>100000</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5">
+        <v>72</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>